<commit_message>
model changes and new tests
</commit_message>
<xml_diff>
--- a/results-Akram (2022) Aggregate oil prices.xlsx
+++ b/results-Akram (2022) Aggregate oil prices.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -458,13 +458,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.9430191170079473</v>
+        <v>0.9430191170079472</v>
       </c>
       <c r="C2" t="n">
         <v>0.9997049110292087</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2062083391007635</v>
+        <v>0.2062083391007637</v>
       </c>
       <c r="E2" t="inlineStr"/>
     </row>
@@ -504,7 +504,7 @@
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="n">
-        <v>-0.01940808605252104</v>
+        <v>-0.01940808605252101</v>
       </c>
     </row>
     <row r="6">
@@ -517,7 +517,7 @@
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="n">
-        <v>-0.03082886858449932</v>
+        <v>-0.03082886858449931</v>
       </c>
     </row>
   </sheetData>

</xml_diff>